<commit_message>
resolvido a coluna mes e ano
</commit_message>
<xml_diff>
--- a/planilha-mari-5/TIN Collaboration teste 2.xlsx
+++ b/planilha-mari-5/TIN Collaboration teste 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\consolidar-planilha-weg\planilha-mari-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623819DD-1A95-45C9-B44A-0A84C79DF25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B577A975-261C-4E01-A4D7-6CA6E31F87CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -310,7 +310,7 @@
     <t>kkkkkkkkkkkkkkkkkkkkkkkkkkk</t>
   </si>
   <si>
-    <t>mar/252</t>
+    <t>mar/26</t>
   </si>
 </sst>
 </file>
@@ -2359,7 +2359,7 @@
     <tableColumn id="25" xr3:uid="{C5C6F9DA-C654-4668-9412-C46C2E27CCB5}" name="dez/25" dataDxfId="194"/>
     <tableColumn id="17" xr3:uid="{B00F94A8-6EA1-4A54-B1C0-9BAF7B1B236C}" name="jan/26" dataDxfId="193"/>
     <tableColumn id="27" xr3:uid="{8C9FB46B-37EF-4485-9F51-6E4030143374}" name="fev/26" dataDxfId="192"/>
-    <tableColumn id="28" xr3:uid="{FA13D833-8A99-4ED4-BF00-BBD42CFE6F02}" name="mar/252" dataDxfId="0"/>
+    <tableColumn id="28" xr3:uid="{E3FE6030-8DE0-4359-B4A0-25451CBC36D0}" name="mar/26" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3874,7 +3874,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA20" sqref="AA20"/>
+      <selection pane="bottomLeft" activeCell="AA2" sqref="AA2:AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3889,7 +3889,7 @@
     <col min="8" max="8" width="10.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
     <col min="10" max="25" width="11.5703125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="8.5703125" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -11234,6 +11234,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010055299C8A5E56DF42BB3A496FAB31A3CA" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="f48546ee30a9c08b8c56cc99cae99613">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="886f8626-7949-4fe5-8403-a629ca357b95" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4da67acbd85d4947d1135fd4f9dd5422" ns2:_="">
     <xsd:import namespace="886f8626-7949-4fe5-8403-a629ca357b95"/>
@@ -11377,12 +11383,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1C848C-A0C9-41E4-8BB1-646104CE90D9}">
   <ds:schemaRefs>
@@ -11392,6 +11392,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076963EF-7E18-4286-B416-ADA05C6F6E23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64AD39B2-FED1-46F1-B570-2B06EBE1DD70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11409,15 +11418,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076963EF-7E18-4286-B416-ADA05C6F6E23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{886666a6-a8d2-4604-a002-95b622cb7e18}" enabled="0" method="" siteId="{886666a6-a8d2-4604-a002-95b622cb7e18}" removed="1"/>

</xml_diff>